<commit_message>
Configured Mail with attachments
</commit_message>
<xml_diff>
--- a/InsuranceClaimAutomation - UiPATH/ClaimData.xlsx
+++ b/InsuranceClaimAutomation - UiPATH/ClaimData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>TN 49 B6666</t>
   </si>
@@ -128,6 +128,36 @@
   </si>
   <si>
     <t>Nellore</t>
+  </si>
+  <si>
+    <t>DL 26 K 0001</t>
+  </si>
+  <si>
+    <t>RAMSON</t>
+  </si>
+  <si>
+    <t>65, Rajpath,, Connaught</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
+    <t>ramson23@gmail.com</t>
+  </si>
+  <si>
+    <t>Agra</t>
+  </si>
+  <si>
+    <t>Severe Damage</t>
+  </si>
+  <si>
+    <t>RAGAV</t>
+  </si>
+  <si>
+    <t>TN38BXY8896668</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -473,7 +503,7 @@
   <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:T8"/>
+      <selection activeCell="E6" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,8 +751,66 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J5" s="1"/>
-      <c r="T5" s="1"/>
+      <c r="A5">
+        <v>9965665</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5">
+        <v>100001</v>
+      </c>
+      <c r="G5">
+        <v>2147483647</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5">
+        <v>60</v>
+      </c>
+      <c r="P5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>9</v>
+      </c>
+      <c r="R5" t="s">
+        <v>19</v>
+      </c>
+      <c r="S5" t="s">
+        <v>47</v>
+      </c>
+      <c r="T5" s="1">
+        <v>43129.550312500003</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="J6" s="1"/>

</xml_diff>